<commit_message>
Updates to 3.5 documentation post release (#1158)
* Post 3.5 launch fixes

* Integrate filtered HTML Model Zoo
</commit_message>
<xml_diff>
--- a/docs/_downloads/ff9554ff9ff6240811c20ede15113dbd/ModelZoo_Github.xlsx
+++ b/docs/_downloads/ff9554ff9ff6240811c20ede15113dbd/ModelZoo_Github.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\vitis-ai-staging\docsrc\source\docs\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28D1299B-06B6-4ECA-9ED5-CA546B84F694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B78BE58-FC16-4D36-83B5-528EE33229ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{FDEDB1A0-B1D7-4FF6-B821-F3B34B308466}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="381">
   <si>
     <t>Task</t>
   </si>
@@ -819,17 +819,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>E2E throughput (fps) 
-Single Thread</t>
-  </si>
-  <si>
-    <t>E2E throughput (fps) 
-Multi Thread</t>
-  </si>
-  <si>
-    <t>4PE DPUCVDX8H @350MHz Gen4x8</t>
-  </si>
-  <si>
     <t>Non-Commercial Use Only</t>
   </si>
   <si>
@@ -1300,15 +1289,6 @@
   </si>
   <si>
     <t>Copyleft Model Zoo</t>
-  </si>
-  <si>
-    <t>V70</t>
-  </si>
-  <si>
-    <t>VEK280</t>
-  </si>
-  <si>
-    <t>1* C20B14CU1 @ 300MHz</t>
   </si>
   <si>
     <t>/</t>
@@ -1358,6 +1338,27 @@
       </rPr>
       <t>Copyright 2023 Advanced Micro Devices, Inc.</t>
     </r>
+  </si>
+  <si>
+    <t>V70
+E2E throughput (fps) 
+Multi Thread
+1* C20B14CU1 @250MHz Gen4x8
+AIE-ML fclk=1.00GHz</t>
+  </si>
+  <si>
+    <t>VEK280
+E2E throughput (fps) 
+Multi Thread
+1* C20B14CU1 @300MHz
+AIE-ML fclk=1.18GHz</t>
+  </si>
+  <si>
+    <t>VEK280
+E2E throughput (fps) 
+Single Thread
+1* C20B14CU1 @ 300MHz
+AIE-ML fclk=1.18GHz</t>
   </si>
 </sst>
 </file>
@@ -1421,7 +1422,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1433,32 +1434,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -1484,7 +1459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1564,29 +1539,26 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1910,7 +1882,7 @@
       <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S38" sqref="S38"/>
+      <selection pane="bottomRight" activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1935,42 +1907,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="R1" s="31" t="s">
-        <v>376</v>
-      </c>
-      <c r="S1" s="32"/>
-      <c r="T1" s="34" t="s">
-        <v>375</v>
-      </c>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="31"/>
     </row>
     <row r="2" spans="1:20" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
-        <v>383</v>
-      </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="R2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>377</v>
       </c>
-      <c r="S2" s="30"/>
-      <c r="T2" s="34" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="34"/>
+    </row>
+    <row r="3" spans="1:20" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1987,10 +1951,10 @@
         <v>4</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>5</v>
@@ -2019,17 +1983,17 @@
       <c r="P3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="35" t="s">
+      <c r="Q3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="R3" s="23" t="s">
-        <v>252</v>
+        <v>380</v>
       </c>
       <c r="S3" s="23" t="s">
-        <v>253</v>
+        <v>379</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>253</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
@@ -2046,11 +2010,11 @@
         <v>29</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>218</v>
@@ -2079,13 +2043,13 @@
       <c r="P4" s="14"/>
       <c r="Q4" s="15"/>
       <c r="R4" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S4" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T4" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
@@ -2100,11 +2064,11 @@
         <v>29</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>211</v>
@@ -2133,13 +2097,13 @@
       <c r="P5" s="14"/>
       <c r="Q5" s="15"/>
       <c r="R5" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S5" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T5" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
@@ -2154,11 +2118,11 @@
         <v>29</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>211</v>
@@ -2187,13 +2151,13 @@
       <c r="P6" s="14"/>
       <c r="Q6" s="15"/>
       <c r="R6" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S6" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T6" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
@@ -2208,11 +2172,11 @@
         <v>29</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>211</v>
@@ -2241,13 +2205,13 @@
       <c r="P7" s="14"/>
       <c r="Q7" s="15"/>
       <c r="R7" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S7" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T7" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
@@ -2264,23 +2228,23 @@
         <v>29</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="11" t="s">
+        <v>370</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>376</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="K8" s="27" t="s">
         <v>373</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>381</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>382</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>380</v>
-      </c>
-      <c r="K8" s="33" t="s">
-        <v>379</v>
       </c>
       <c r="L8" s="11" t="s">
         <v>159</v>
@@ -2320,11 +2284,11 @@
         <v>29</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F9" s="19"/>
       <c r="G9" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>163</v>
@@ -2355,13 +2319,13 @@
       </c>
       <c r="Q9" s="15"/>
       <c r="R9" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S9" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T9" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
@@ -2378,11 +2342,11 @@
         <v>29</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>163</v>
@@ -2411,13 +2375,13 @@
       <c r="P10" s="14"/>
       <c r="Q10" s="15"/>
       <c r="R10" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S10" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T10" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
@@ -2434,11 +2398,11 @@
         <v>29</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>245</v>
@@ -2475,7 +2439,7 @@
         <v>16.681899999999999</v>
       </c>
       <c r="T11" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
@@ -2492,11 +2456,11 @@
         <v>29</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F12" s="19"/>
       <c r="G12" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>245</v>
@@ -2531,7 +2495,7 @@
         <v>19.1465</v>
       </c>
       <c r="T12" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
@@ -2548,11 +2512,11 @@
         <v>29</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>227</v>
@@ -2581,13 +2545,13 @@
       <c r="P13" s="14"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S13" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T13" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
@@ -2602,13 +2566,13 @@
         <v>29</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>22</v>
@@ -2660,13 +2624,13 @@
         <v>29</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>22</v>
@@ -2718,13 +2682,13 @@
         <v>29</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>22</v>
@@ -2776,13 +2740,13 @@
         <v>29</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>22</v>
@@ -2834,13 +2798,13 @@
         <v>29</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>22</v>
@@ -2892,11 +2856,11 @@
         <v>29</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>239</v>
@@ -2946,13 +2910,13 @@
         <v>29</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>26</v>
@@ -3004,11 +2968,11 @@
         <v>29</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>193</v>
@@ -3056,13 +3020,13 @@
         <v>29</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>26</v>
@@ -3114,13 +3078,13 @@
         <v>29</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>26</v>
@@ -3172,13 +3136,13 @@
         <v>29</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>26</v>
@@ -3230,13 +3194,13 @@
         <v>29</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>26</v>
@@ -3288,13 +3252,13 @@
         <v>29</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>26</v>
@@ -3323,13 +3287,13 @@
       <c r="P26" s="14"/>
       <c r="Q26" s="15"/>
       <c r="R26" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S26" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T26" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.35">
@@ -3344,11 +3308,11 @@
         <v>29</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>129</v>
@@ -3398,11 +3362,11 @@
         <v>29</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F28" s="19"/>
       <c r="G28" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H28" s="12" t="s">
         <v>129</v>
@@ -3452,11 +3416,11 @@
         <v>29</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F29" s="19"/>
       <c r="G29" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>129</v>
@@ -3506,11 +3470,11 @@
         <v>29</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F30" s="19"/>
       <c r="G30" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>134</v>
@@ -3562,11 +3526,11 @@
         <v>29</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F31" s="19"/>
       <c r="G31" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>173</v>
@@ -3597,13 +3561,13 @@
       </c>
       <c r="Q31" s="15"/>
       <c r="R31" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S31" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T31" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.35">
@@ -3618,13 +3582,13 @@
         <v>29</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>26</v>
@@ -3676,13 +3640,13 @@
         <v>29</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>26</v>
@@ -3734,13 +3698,13 @@
         <v>29</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>26</v>
@@ -3792,13 +3756,13 @@
         <v>29</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H35" s="12" t="s">
         <v>26</v>
@@ -3850,13 +3814,13 @@
         <v>29</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H36" s="12" t="s">
         <v>26</v>
@@ -3908,13 +3872,13 @@
         <v>29</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H37" s="12" t="s">
         <v>26</v>
@@ -3966,11 +3930,11 @@
         <v>29</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F38" s="19"/>
       <c r="G38" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H38" s="12" t="s">
         <v>199</v>
@@ -4020,13 +3984,13 @@
         <v>29</v>
       </c>
       <c r="E39" s="19" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H39" s="12" t="s">
         <v>27</v>
@@ -4078,11 +4042,11 @@
         <v>29</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F40" s="19"/>
       <c r="G40" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>67</v>
@@ -4134,11 +4098,11 @@
         <v>29</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F41" s="19"/>
       <c r="G41" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H41" s="12" t="s">
         <v>67</v>
@@ -4190,11 +4154,11 @@
         <v>29</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F42" s="19"/>
       <c r="G42" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H42" s="12" t="s">
         <v>67</v>
@@ -4246,11 +4210,11 @@
         <v>29</v>
       </c>
       <c r="E43" s="19" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F43" s="19"/>
       <c r="G43" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H43" s="12" t="s">
         <v>67</v>
@@ -4279,13 +4243,13 @@
       <c r="P43" s="14"/>
       <c r="Q43" s="15"/>
       <c r="R43" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S43" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T43" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.35">
@@ -4300,11 +4264,11 @@
         <v>29</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F44" s="19"/>
       <c r="G44" s="11" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="H44" s="12" t="s">
         <v>137</v>
@@ -4354,11 +4318,11 @@
         <v>29</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F45" s="19"/>
       <c r="G45" s="11" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="H45" s="12" t="s">
         <v>140</v>
@@ -4408,11 +4372,11 @@
         <v>29</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F46" s="19"/>
       <c r="G46" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H46" s="12" t="s">
         <v>144</v>
@@ -4462,14 +4426,14 @@
         <v>29</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F47" s="19"/>
       <c r="G47" s="11" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I47" s="21"/>
       <c r="J47" s="18" t="s">
@@ -4502,7 +4466,7 @@
         <v>78.078299999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48" s="12" t="s">
         <v>209</v>
       </c>
@@ -4514,11 +4478,11 @@
         <v>70</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F48" s="19"/>
       <c r="G48" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H48" s="12" t="s">
         <v>211</v>
@@ -4547,13 +4511,13 @@
       <c r="P48" s="14"/>
       <c r="Q48" s="15"/>
       <c r="R48" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S48" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T48" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.35">
@@ -4568,11 +4532,11 @@
         <v>70</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="F49" s="19"/>
       <c r="G49" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H49" s="12" t="s">
         <v>146</v>
@@ -4601,13 +4565,13 @@
       <c r="P49" s="14"/>
       <c r="Q49" s="15"/>
       <c r="R49" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S49" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T49" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.35">
@@ -4622,13 +4586,13 @@
         <v>70</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H50" s="12" t="s">
         <v>71</v>
@@ -4678,13 +4642,13 @@
         <v>70</v>
       </c>
       <c r="E51" s="19" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="F51" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H51" s="12" t="s">
         <v>76</v>
@@ -4734,13 +4698,13 @@
         <v>70</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H52" s="12" t="s">
         <v>80</v>
@@ -4792,11 +4756,11 @@
         <v>70</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="F53" s="19"/>
       <c r="G53" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H53" s="12" t="s">
         <v>178</v>
@@ -4831,7 +4795,7 @@
         <v>24.039200000000001</v>
       </c>
       <c r="T53" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.35">
@@ -4846,13 +4810,13 @@
         <v>70</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H54" s="12" t="s">
         <v>16</v>
@@ -4904,13 +4868,13 @@
         <v>70</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F55" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H55" s="12" t="s">
         <v>16</v>
@@ -4962,13 +4926,13 @@
         <v>70</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H56" s="12" t="s">
         <v>16</v>
@@ -5018,13 +4982,13 @@
         <v>70</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H57" s="12" t="s">
         <v>22</v>
@@ -5076,13 +5040,13 @@
         <v>70</v>
       </c>
       <c r="E58" s="19" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H58" s="12" t="s">
         <v>22</v>
@@ -5134,13 +5098,13 @@
         <v>70</v>
       </c>
       <c r="E59" s="19" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H59" s="12" t="s">
         <v>22</v>
@@ -5190,13 +5154,13 @@
         <v>70</v>
       </c>
       <c r="E60" s="19" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F60" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H60" s="12" t="s">
         <v>24</v>
@@ -5248,13 +5212,13 @@
         <v>70</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H61" s="12" t="s">
         <v>24</v>
@@ -5306,13 +5270,13 @@
         <v>70</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H62" s="12" t="s">
         <v>24</v>
@@ -5362,11 +5326,11 @@
         <v>70</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F63" s="19"/>
       <c r="G63" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H63" s="12" t="s">
         <v>149</v>
@@ -5418,13 +5382,13 @@
         <v>70</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H64" s="12" t="s">
         <v>26</v>
@@ -5476,13 +5440,13 @@
         <v>70</v>
       </c>
       <c r="E65" s="19" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H65" s="12" t="s">
         <v>90</v>
@@ -5532,13 +5496,13 @@
         <v>70</v>
       </c>
       <c r="E66" s="19" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H66" s="12" t="s">
         <v>90</v>
@@ -5590,13 +5554,13 @@
         <v>70</v>
       </c>
       <c r="E67" s="19" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H67" s="12" t="s">
         <v>90</v>
@@ -5648,13 +5612,13 @@
         <v>70</v>
       </c>
       <c r="E68" s="19" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="F68" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H68" s="12" t="s">
         <v>90</v>
@@ -5704,13 +5668,13 @@
         <v>70</v>
       </c>
       <c r="E69" s="19" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F69" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H69" s="12" t="s">
         <v>93</v>
@@ -5760,13 +5724,13 @@
         <v>70</v>
       </c>
       <c r="E70" s="19" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F70" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H70" s="12" t="s">
         <v>93</v>
@@ -5804,7 +5768,7 @@
         <v>8081.16</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A71" s="12" t="s">
         <v>192</v>
       </c>
@@ -5818,11 +5782,11 @@
         <v>70</v>
       </c>
       <c r="E71" s="19" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F71" s="19"/>
       <c r="G71" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H71" s="12" t="s">
         <v>205</v>
@@ -5876,11 +5840,11 @@
         <v>70</v>
       </c>
       <c r="E72" s="19" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F72" s="19"/>
       <c r="G72" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H72" s="12" t="s">
         <v>151</v>
@@ -5892,7 +5856,7 @@
         <v>155</v>
       </c>
       <c r="K72" s="16" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="L72" s="17" t="s">
         <v>122</v>
@@ -5934,11 +5898,11 @@
         <v>70</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F73" s="19"/>
       <c r="G73" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H73" s="12" t="s">
         <v>151</v>
@@ -5950,7 +5914,7 @@
         <v>155</v>
       </c>
       <c r="K73" s="16" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="L73" s="17" t="s">
         <v>122</v>
@@ -5992,11 +5956,11 @@
         <v>70</v>
       </c>
       <c r="E74" s="19" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="F74" s="19"/>
       <c r="G74" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H74" s="12" t="s">
         <v>151</v>
@@ -6008,7 +5972,7 @@
         <v>155</v>
       </c>
       <c r="K74" s="16" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="L74" s="17" t="s">
         <v>122</v>
@@ -6050,11 +6014,11 @@
         <v>70</v>
       </c>
       <c r="E75" s="19" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="F75" s="19"/>
       <c r="G75" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H75" s="12" t="s">
         <v>151</v>
@@ -6066,7 +6030,7 @@
         <v>155</v>
       </c>
       <c r="K75" s="16" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="L75" s="17" t="s">
         <v>122</v>
@@ -6108,11 +6072,11 @@
         <v>70</v>
       </c>
       <c r="E76" s="19" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F76" s="19"/>
       <c r="G76" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H76" s="12" t="s">
         <v>151</v>
@@ -6124,7 +6088,7 @@
         <v>155</v>
       </c>
       <c r="K76" s="16" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="L76" s="17" t="s">
         <v>122</v>
@@ -6162,13 +6126,13 @@
         <v>70</v>
       </c>
       <c r="E77" s="19" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H77" s="12" t="s">
         <v>94</v>
@@ -6220,13 +6184,13 @@
         <v>70</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H78" s="12" t="s">
         <v>94</v>
@@ -6278,13 +6242,13 @@
         <v>70</v>
       </c>
       <c r="E79" s="19" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F79" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H79" s="12" t="s">
         <v>26</v>
@@ -6334,13 +6298,13 @@
         <v>70</v>
       </c>
       <c r="E80" s="19" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H80" s="12" t="s">
         <v>97</v>
@@ -6392,13 +6356,13 @@
         <v>70</v>
       </c>
       <c r="E81" s="19" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F81" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H81" s="12" t="s">
         <v>97</v>
@@ -6450,13 +6414,13 @@
         <v>70</v>
       </c>
       <c r="E82" s="19" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="F82" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H82" s="12" t="s">
         <v>26</v>
@@ -6506,13 +6470,13 @@
         <v>70</v>
       </c>
       <c r="E83" s="19" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F83" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H83" s="12" t="s">
         <v>26</v>
@@ -6564,13 +6528,13 @@
         <v>70</v>
       </c>
       <c r="E84" s="19" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F84" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H84" s="12" t="s">
         <v>26</v>
@@ -6622,13 +6586,13 @@
         <v>70</v>
       </c>
       <c r="E85" s="19" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F85" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G85" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H85" s="12" t="s">
         <v>26</v>
@@ -6678,13 +6642,13 @@
         <v>70</v>
       </c>
       <c r="E86" s="19" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F86" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H86" s="12" t="s">
         <v>100</v>
@@ -6734,13 +6698,13 @@
         <v>70</v>
       </c>
       <c r="E87" s="19" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H87" s="12" t="s">
         <v>100</v>
@@ -6790,13 +6754,13 @@
         <v>70</v>
       </c>
       <c r="E88" s="19" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H88" s="12" t="s">
         <v>100</v>
@@ -6846,11 +6810,11 @@
         <v>70</v>
       </c>
       <c r="E89" s="19" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F89" s="19"/>
       <c r="G89" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H89" s="12" t="s">
         <v>156</v>
@@ -6900,11 +6864,11 @@
         <v>70</v>
       </c>
       <c r="E90" s="19" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F90" s="19"/>
       <c r="G90" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H90" s="12" t="s">
         <v>157</v>
@@ -6954,11 +6918,11 @@
         <v>70</v>
       </c>
       <c r="E91" s="19" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="F91" s="19"/>
       <c r="G91" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H91" s="12" t="s">
         <v>186</v>
@@ -6993,7 +6957,7 @@
         <v>123.68300000000001</v>
       </c>
       <c r="T91" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.35">
@@ -7008,13 +6972,13 @@
         <v>70</v>
       </c>
       <c r="E92" s="19" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F92" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H92" s="12" t="s">
         <v>102</v>
@@ -7066,13 +7030,13 @@
         <v>70</v>
       </c>
       <c r="E93" s="19" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F93" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H93" s="12" t="s">
         <v>102</v>
@@ -7124,13 +7088,13 @@
         <v>70</v>
       </c>
       <c r="E94" s="19" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F94" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H94" s="12" t="s">
         <v>102</v>
@@ -7180,13 +7144,13 @@
         <v>70</v>
       </c>
       <c r="E95" s="19" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F95" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G95" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H95" s="12" t="s">
         <v>104</v>
@@ -7238,13 +7202,13 @@
         <v>70</v>
       </c>
       <c r="E96" s="19" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F96" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G96" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H96" s="12" t="s">
         <v>104</v>
@@ -7294,13 +7258,13 @@
         <v>70</v>
       </c>
       <c r="E97" s="19" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F97" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H97" s="12" t="s">
         <v>104</v>
@@ -7350,13 +7314,13 @@
         <v>70</v>
       </c>
       <c r="E98" s="19" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F98" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G98" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H98" s="12" t="s">
         <v>107</v>
@@ -7385,13 +7349,13 @@
       <c r="P98" s="14"/>
       <c r="Q98" s="15"/>
       <c r="R98" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S98" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T98" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.35">
@@ -7406,11 +7370,11 @@
         <v>70</v>
       </c>
       <c r="E99" s="19" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F99" s="19"/>
       <c r="G99" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H99" s="12" t="s">
         <v>123</v>
@@ -7460,11 +7424,11 @@
         <v>70</v>
       </c>
       <c r="E100" s="19" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="F100" s="19"/>
       <c r="G100" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H100" s="12" t="s">
         <v>158</v>
@@ -7514,11 +7478,11 @@
         <v>70</v>
       </c>
       <c r="E101" s="19" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F101" s="19"/>
       <c r="G101" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H101" s="12" t="s">
         <v>158</v>
@@ -7568,13 +7532,13 @@
         <v>110</v>
       </c>
       <c r="E102" s="19" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F102" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G102" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H102" s="12" t="s">
         <v>111</v>
@@ -7603,13 +7567,13 @@
       <c r="P102" s="14"/>
       <c r="Q102" s="15"/>
       <c r="R102" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S102" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T102" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.35">
@@ -7624,13 +7588,13 @@
         <v>110</v>
       </c>
       <c r="E103" s="19" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F103" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G103" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H103" s="12" t="s">
         <v>115</v>
@@ -7678,13 +7642,13 @@
         <v>110</v>
       </c>
       <c r="E104" s="19" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F104" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G104" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H104" s="12" t="s">
         <v>22</v>
@@ -7734,13 +7698,13 @@
         <v>110</v>
       </c>
       <c r="E105" s="19" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F105" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G105" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H105" s="12" t="s">
         <v>90</v>
@@ -7790,13 +7754,13 @@
         <v>110</v>
       </c>
       <c r="E106" s="19" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F106" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G106" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H106" s="12" t="s">
         <v>117</v>
@@ -7825,13 +7789,13 @@
       <c r="P106" s="14"/>
       <c r="Q106" s="15"/>
       <c r="R106" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="S106" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="T106" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.35">
@@ -7846,13 +7810,13 @@
         <v>110</v>
       </c>
       <c r="E107" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F107" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G107" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H107" s="12" t="s">
         <v>26</v>
@@ -7902,11 +7866,11 @@
         <v>110</v>
       </c>
       <c r="E108" s="19" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F108" s="19"/>
       <c r="G108" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H108" s="12" t="s">
         <v>123</v>
@@ -7952,36 +7916,36 @@
         <v>153</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D109" s="12" t="s">
         <v>110</v>
       </c>
       <c r="E109" s="12" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F109" s="12"/>
       <c r="G109" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H109" s="12" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="I109" s="12"/>
       <c r="J109" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="K109" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="L109" s="17" t="s">
+        <v>366</v>
+      </c>
+      <c r="M109" s="17" t="s">
         <v>367</v>
       </c>
-      <c r="K109" s="16" t="s">
+      <c r="N109" s="17" t="s">
         <v>368</v>
-      </c>
-      <c r="L109" s="17" t="s">
-        <v>369</v>
-      </c>
-      <c r="M109" s="17" t="s">
-        <v>370</v>
-      </c>
-      <c r="N109" s="17" t="s">
-        <v>371</v>
       </c>
       <c r="O109" s="17">
         <v>24.6</v>
@@ -8536,6 +8500,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AAFFF3D42354FC46AAF9DDD3E79C50EB" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2dc978867c734327b61f3800eb63d242">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e1d46fbb-7d1a-4672-bfd6-63f33723acfe" xmlns:ns4="5abdcbab-ff3d-4b55-bc16-63963a6146d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c122bff22086de4b34442ce3fa7ec584" ns3:_="" ns4:_="">
     <xsd:import namespace="e1d46fbb-7d1a-4672-bfd6-63f33723acfe"/>
@@ -8764,22 +8743,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7132B4B-6BDC-47A9-AF0C-0341A70E6725}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="e1d46fbb-7d1a-4672-bfd6-63f33723acfe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5abdcbab-ff3d-4b55-bc16-63963a6146d3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{454B4A55-1C62-49DF-B7EA-FD56AEB4B42C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58A6EA98-5C4B-47AC-A15E-1B7C0018A8AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8796,29 +8785,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{454B4A55-1C62-49DF-B7EA-FD56AEB4B42C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7132B4B-6BDC-47A9-AF0C-0341A70E6725}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="e1d46fbb-7d1a-4672-bfd6-63f33723acfe"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5abdcbab-ff3d-4b55-bc16-63963a6146d3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>